<commit_message>
added csv combination script
</commit_message>
<xml_diff>
--- a/results/log_reg_results.xlsx
+++ b/results/log_reg_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Documents/Projekte/Boston Celi/1 Causal Inference/Race Interventions/mit-tmle/results/MIMIC/log_reg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E3A78E-7527-7349-9F8C-B7D9D511DB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49661CCE-C131-8948-9FFA-E506E1995979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIMIC" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -695,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modify way results are saved and add Paper's tables in Excel
</commit_message>
<xml_diff>
--- a/results/log_reg_results.xlsx
+++ b/results/log_reg_results.xlsx
@@ -1,27 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\Race Disparities in Sepsis\mit-tmle\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49661CCE-C131-8948-9FFA-E506E1995979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691B479B-B220-4241-ABE0-88877B86CBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIMIC" sheetId="1" r:id="rId1"/>
     <sheet name="eICU" sheetId="2" r:id="rId2"/>
+    <sheet name="processed" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
   <si>
     <t>SOFA</t>
   </si>
@@ -57,16 +71,99 @@
   </si>
   <si>
     <t>vasopressor all</t>
+  </si>
+  <si>
+    <t>0 - 5</t>
+  </si>
+  <si>
+    <t>6 - 10</t>
+  </si>
+  <si>
+    <t>11 - 15</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>vent</t>
+  </si>
+  <si>
+    <t>rrt</t>
+  </si>
+  <si>
+    <t>vasopressor</t>
+  </si>
+  <si>
+    <t>OR_uCI</t>
+  </si>
+  <si>
+    <t>OR_iCI</t>
+  </si>
+  <si>
+    <t>&gt; 15</t>
+  </si>
+  <si>
+    <t>Ventilation</t>
+  </si>
+  <si>
+    <t>RRT</t>
+  </si>
+  <si>
+    <t>Vasopressor</t>
+  </si>
+  <si>
+    <t>SOFA Ranges</t>
+  </si>
+  <si>
+    <t>MIMIC</t>
+  </si>
+  <si>
+    <t>eICU</t>
+  </si>
+  <si>
+    <t>Cohort</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Odds Ratio (CI)
+ White vs. Non-White</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,14 +186,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -406,15 +548,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScale="183" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="20" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +577,29 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -447,8 +615,53 @@
       <c r="E2" s="1">
         <v>2.0303663723171089E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>4</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2">
+        <v>2</v>
+      </c>
+      <c r="U2" s="2">
+        <v>3</v>
+      </c>
+      <c r="V2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -464,8 +677,56 @@
       <c r="E3" s="1">
         <v>0.15444435746675034</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.0805156270891112</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1.0742570173570762</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.1159681744305328</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.90007262241465258</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1.0594182016464102</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.60545784097768851</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.50018116644710175</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.53474367307389481</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.83402887234041712</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1.1090522236916016</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1.3908299431103659</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1.4157844577619512</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1.4163562342273666</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1.120289564433353</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0.6996862226198759</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -481,8 +742,56 @@
       <c r="E4" s="1">
         <v>2.806363139415519E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.0121096424754867</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.97340089314414813</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.0118811244755381</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.72247449551769238</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.48143330738577345</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.55132560673533748</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.40244925346720251</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.46817724482810263</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.69594724109511552</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0.75373651493266636</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1.2982740967594486</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1.2743562475779044</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1.2834503189468423</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0.86519066549887136</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0.14604122647145779</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -498,8 +807,56 @@
       <c r="E5" s="1">
         <v>0.34782715586151403</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.1535450028202376</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.1855630577996858</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.2307621282957557</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.1213277847820593</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2.3313030252814619</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.66490508099570156</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0.62164657310955052</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.61077465650333151</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.99950702987607531</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1.6318657919673241</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1.4899842302028163</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1.5729083877840571</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1.5630250369806593</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1.4506036163191929</v>
+      </c>
+      <c r="V5" s="1">
+        <v>3.352209659919215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -515,8 +872,56 @@
       <c r="E6" s="1">
         <v>0.88594598852589046</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.0303663723171089E-2</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.15444435746675034</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2.806363139415519E-2</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.34782715586151403</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.88594598852589046</v>
+      </c>
+      <c r="M6" s="1">
+        <v>8.610201175008081E-26</v>
+      </c>
+      <c r="N6" s="1">
+        <v>4.2178417094128644E-10</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2.738268689919817E-20</v>
+      </c>
+      <c r="P6" s="1">
+        <v>4.9379107472904568E-2</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0.5993976831686606</v>
+      </c>
+      <c r="R6" s="1">
+        <v>6.0397657786188027E-21</v>
+      </c>
+      <c r="S6" s="1">
+        <v>9.4801743458325452E-11</v>
+      </c>
+      <c r="T6" s="1">
+        <v>4.3972584807742551E-12</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0.38891668209609193</v>
+      </c>
+      <c r="V6" s="5">
+        <v>0.65505264725132828</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -533,7 +938,7 @@
         <v>8.610201175008081E-26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -550,7 +955,7 @@
         <v>4.2178417094128644E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -567,7 +972,7 @@
         <v>2.738268689919817E-20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -584,7 +989,7 @@
         <v>4.9379107472904568E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -601,7 +1006,7 @@
         <v>0.5993976831686606</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -618,7 +1023,7 @@
         <v>6.0397657786188027E-21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -635,7 +1040,7 @@
         <v>9.4801743458325452E-11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -652,7 +1057,7 @@
         <v>4.3972584807742551E-12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -669,7 +1074,7 @@
         <v>0.38891668209609193</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -687,24 +1092,29 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="R1:V1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B2" sqref="B2:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -720,8 +1130,29 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -737,8 +1168,53 @@
       <c r="E2" s="1">
         <v>2.1394542774132628E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>4</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2">
+        <v>2</v>
+      </c>
+      <c r="U2" s="2">
+        <v>3</v>
+      </c>
+      <c r="V2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -754,8 +1230,52 @@
       <c r="E3" s="1">
         <v>0.70113122432516373</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.0850809048195786</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.98740278567187356</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.3087197465033948</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.97421519129012579</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <v>0.62843489377879613</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.58425984721053104</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.6174260867232686</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1.0030156715056535</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.98794831451896181</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1.1208200693118302</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1.0933195670849958</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1.1639972501915532</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1.1839428527297362</v>
+      </c>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -771,8 +1291,52 @@
       <c r="E4" s="1">
         <v>4.8371539126914768E-9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.0299671931623935</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.92550337683590744</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.1959600573018645</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.71863670535125446</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1">
+        <v>0.58250158351725478</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.5175082021478673</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.55396225389586273</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.80566086619203692</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0.45832836534475974</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1.0638781706034284</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1.0246453156655433</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1.0636180975997049</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0.82998593327552495</v>
+      </c>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -788,19 +1352,105 @@
       <c r="E5" s="1">
         <v>0.8663716542151364</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.1431437601318204</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.0534421435454555</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.4321108505512627</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.3206885090520928</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1">
+        <v>0.67799028688317409</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0.65962156279976514</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.68816055585995273</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1.248714539209278</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>2.1295689858223543</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1.1808096664485952</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1.1665965358895942</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1.2738497036775818</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1.6888487169872382</v>
+      </c>
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.1394542774132628E-3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.70113122432516373</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4.8371539126914768E-9</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.8663716542151364</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1">
+        <v>3.7614586814981702E-33</v>
+      </c>
+      <c r="N6" s="1">
+        <v>3.888977497180045E-18</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2.9473185237582918E-18</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0.97851099567074218</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.97531628674358151</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1.8060824641937391E-5</v>
+      </c>
+      <c r="S6" s="1">
+        <v>7.0274651563082564E-3</v>
+      </c>
+      <c r="T6" s="1">
+        <v>9.6554055855737893E-4</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0.3514863588822163</v>
+      </c>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -817,7 +1467,7 @@
         <v>3.7614586814981702E-33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -834,7 +1484,7 @@
         <v>3.888977497180045E-18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -851,7 +1501,7 @@
         <v>2.9473185237582918E-18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -868,7 +1518,7 @@
         <v>0.97851099567074218</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -885,7 +1535,7 @@
         <v>0.97531628674358151</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -902,7 +1552,7 @@
         <v>1.8060824641937391E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -919,7 +1569,7 @@
         <v>7.0274651563082564E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -936,7 +1586,7 @@
         <v>9.6554055855737893E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -953,12 +1603,245 @@
         <v>0.3514863588822163</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="R1:V1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72440BF3-33B5-4D9D-850C-0A4456E13577}">
+  <dimension ref="A3:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="196" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!H3, 2), " (", ROUND(MIMIC!H4,2), " - ", ROUND(MIMIC!H5,2),  ")", IF(AND(MIMIC!H6 &lt;0.05, NOT(ISBLANK(MIMIC!H6))), "*", " ") )</f>
+        <v>1.08 (1.01 - 1.15)*</v>
+      </c>
+      <c r="D5" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!I3, 2), " (", ROUND(MIMIC!I4,2), " - ", ROUND(MIMIC!I5,2),  ")", IF(AND(MIMIC!I6 &lt;0.05, NOT(ISBLANK(MIMIC!I6))), "*", " ") )</f>
+        <v xml:space="preserve">1.07 (0.97 - 1.19) </v>
+      </c>
+      <c r="E5" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!J3, 2), " (", ROUND(MIMIC!J4,2), " - ", ROUND(MIMIC!J5,2),  ")", IF(AND(MIMIC!J6 &lt;0.05, NOT(ISBLANK(MIMIC!J6))), "*", " ") )</f>
+        <v>1.12 (1.01 - 1.23)*</v>
+      </c>
+      <c r="F5" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!K3, 2), " (", ROUND(MIMIC!K4,2), " - ", ROUND(MIMIC!K5,2),  ")", IF(AND(MIMIC!K6 &lt;0.05, NOT(ISBLANK(MIMIC!K6))), "*", " ") )</f>
+        <v xml:space="preserve">0.9 (0.72 - 1.12) </v>
+      </c>
+      <c r="G5" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!L3, 2), " (", ROUND(MIMIC!L4,2), " - ", ROUND(MIMIC!L5,2),  ")", IF(AND(MIMIC!L6 &lt;0.05, NOT(ISBLANK(MIMIC!L6))), "*", " ") )</f>
+        <v xml:space="preserve">1.06 (0.48 - 2.33) </v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!H3, 2), " (", ROUND(eICU!H4,2), " - ", ROUND(eICU!H5,2),  ")", IF(AND(eICU!H6 &lt;0.05, NOT(ISBLANK(eICU!H6))), "*", " ") )</f>
+        <v>1.09 (1.03 - 1.14)*</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!I3, 2), " (", ROUND(eICU!I4,2), " - ", ROUND(eICU!I5,2),  ")", IF(AND(eICU!I6 &lt;0.05, NOT(ISBLANK(eICU!I6))), "*", " ") )</f>
+        <v xml:space="preserve">0.99 (0.93 - 1.05) </v>
+      </c>
+      <c r="E6" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!J3, 2), " (", ROUND(eICU!J4,2), " - ", ROUND(eICU!J5,2),  ")", IF(AND(eICU!J6 &lt;0.05, NOT(ISBLANK(eICU!J6))), "*", " ") )</f>
+        <v>1.31 (1.2 - 1.43)*</v>
+      </c>
+      <c r="F6" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!K3, 2), " (", ROUND(eICU!K4,2), " - ", ROUND(eICU!K5,2),  ")", IF(AND(eICU!K6 &lt;0.05, NOT(ISBLANK(eICU!K6))), "*", " ") )</f>
+        <v xml:space="preserve">0.97 (0.72 - 1.32) </v>
+      </c>
+      <c r="G6" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!L3, 2), " (", ROUND(eICU!L4,2), " - ", ROUND(eICU!L5,2),  ")", IF(AND(eICU!L6 &lt;0.05, NOT(ISBLANK(eICU!L6))), "*", " ") )</f>
+        <v xml:space="preserve">0 (0 - 0) </v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!M3, 2), " (", ROUND(MIMIC!M4,2), " - ", ROUND(MIMIC!M5,2),  ")", IF(AND(MIMIC!M6 &lt;0.05, NOT(ISBLANK(MIMIC!M6))), "*", " ") )</f>
+        <v>0.61 (0.55 - 0.66)*</v>
+      </c>
+      <c r="D7" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!N3, 2), " (", ROUND(MIMIC!N4,2), " - ", ROUND(MIMIC!N5,2),  ")", IF(AND(MIMIC!N6 &lt;0.05, NOT(ISBLANK(MIMIC!N6))), "*", " ") )</f>
+        <v>0.5 (0.4 - 0.62)*</v>
+      </c>
+      <c r="E7" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!O3, 2), " (", ROUND(MIMIC!O4,2), " - ", ROUND(MIMIC!O5,2),  ")", IF(AND(MIMIC!O6 &lt;0.05, NOT(ISBLANK(MIMIC!O6))), "*", " ") )</f>
+        <v>0.53 (0.47 - 0.61)*</v>
+      </c>
+      <c r="F7" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!P3, 2), " (", ROUND(MIMIC!P4,2), " - ", ROUND(MIMIC!P5,2),  ")", IF(AND(MIMIC!P6 &lt;0.05, NOT(ISBLANK(MIMIC!P6))), "*", " ") )</f>
+        <v>0.83 (0.7 - 1)*</v>
+      </c>
+      <c r="G7" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!Q3, 2), " (", ROUND(MIMIC!Q4,2), " - ", ROUND(MIMIC!Q5,2),  ")", IF(AND(MIMIC!Q6 &lt;0.05, NOT(ISBLANK(MIMIC!Q6))), "*", " ") )</f>
+        <v xml:space="preserve">1.11 (0.75 - 1.63) </v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!M3, 2), " (", ROUND(eICU!M4,2), " - ", ROUND(eICU!M5,2),  ")",, IF(AND(eICU!M6 &lt;0.05, NOT(ISBLANK(eICU!M6))), "*", " ") )</f>
+        <v>0.63 (0.58 - 0.68)*</v>
+      </c>
+      <c r="D8" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!N3, 2), " (", ROUND(eICU!N4,2), " - ", ROUND(eICU!N5,2),  ")",, IF(AND(eICU!N6 &lt;0.05, NOT(ISBLANK(eICU!N6))), "*", " ") )</f>
+        <v>0.58 (0.52 - 0.66)*</v>
+      </c>
+      <c r="E8" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!O3, 2), " (", ROUND(eICU!O4,2), " - ", ROUND(eICU!O5,2),  ")",, IF(AND(eICU!O6 &lt;0.05, NOT(ISBLANK(eICU!O6))), "*", " ") )</f>
+        <v>0.62 (0.55 - 0.69)*</v>
+      </c>
+      <c r="F8" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!P3, 2), " (", ROUND(eICU!P4,2), " - ", ROUND(eICU!P5,2),  ")",, IF(AND(eICU!P6 &lt;0.05, NOT(ISBLANK(eICU!P6))), "*", " ") )</f>
+        <v xml:space="preserve">1 (0.81 - 1.25) </v>
+      </c>
+      <c r="G8" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!Q3, 2), " (", ROUND(eICU!Q4,2), " - ", ROUND(eICU!Q5,2),  ")",, IF(AND(eICU!Q6 &lt;0.05, NOT(ISBLANK(eICU!Q6))), "*", " ") )</f>
+        <v xml:space="preserve">0.99 (0.46 - 2.13) </v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!R3, 2), " (", ROUND(MIMIC!R4,2), " - ", ROUND(MIMIC!R5,2),  ")", IF(AND(MIMIC!R6 &lt;0.05, NOT(ISBLANK(MIMIC!R6))), "*", " ") )</f>
+        <v>1.39 (1.3 - 1.49)*</v>
+      </c>
+      <c r="D9" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!S3, 2), " (", ROUND(MIMIC!S4,2), " - ", ROUND(MIMIC!S5,2),  ")", IF(AND(MIMIC!S6 &lt;0.05, NOT(ISBLANK(MIMIC!S6))), "*", " ") )</f>
+        <v>1.42 (1.27 - 1.57)*</v>
+      </c>
+      <c r="E9" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!T3, 2), " (", ROUND(MIMIC!T4,2), " - ", ROUND(MIMIC!T5,2),  ")", IF(AND(MIMIC!T6 &lt;0.05, NOT(ISBLANK(MIMIC!T6))), "*", " ") )</f>
+        <v>1.42 (1.28 - 1.56)*</v>
+      </c>
+      <c r="F9" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!U3, 2), " (", ROUND(MIMIC!U4,2), " - ", ROUND(MIMIC!U5,2),  ")", IF(AND(MIMIC!U6 &lt;0.05, NOT(ISBLANK(MIMIC!U6))), "*", " ") )</f>
+        <v xml:space="preserve">1.12 (0.87 - 1.45) </v>
+      </c>
+      <c r="G9" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(MIMIC!V3, 2), " (", ROUND(MIMIC!V4,2), " - ", ROUND(MIMIC!V5,2),  ")", IF(AND(MIMIC!V6 &lt;0.05, NOT(ISBLANK(MIMIC!V6))), "*", " ") )</f>
+        <v xml:space="preserve">0.7 (0.15 - 3.35) </v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!R3, 2), " (", ROUND(eICU!R4,2), " - ", ROUND(eICU!R5,2),  ")",, IF(AND(eICU!R6 &lt;0.05, NOT(ISBLANK(eICU!R6))), "*", " ") )</f>
+        <v>1.12 (1.06 - 1.18)*</v>
+      </c>
+      <c r="D10" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!S3, 2), " (", ROUND(eICU!S4,2), " - ", ROUND(eICU!S5,2),  ")",, IF(AND(eICU!S6 &lt;0.05, NOT(ISBLANK(eICU!S6))), "*", " ") )</f>
+        <v>1.09 (1.02 - 1.17)*</v>
+      </c>
+      <c r="E10" s="10" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!T3, 2), " (", ROUND(eICU!T4,2), " - ", ROUND(eICU!T5,2),  ")",, IF(AND(eICU!T6 &lt;0.05, NOT(ISBLANK(eICU!T6))), "*", " ") )</f>
+        <v>1.16 (1.06 - 1.27)*</v>
+      </c>
+      <c r="F10" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!U3, 2), " (", ROUND(eICU!U4,2), " - ", ROUND(eICU!U5,2),  ")",, IF(AND(eICU!U6 &lt;0.05, NOT(ISBLANK(eICU!U6))), "*", " ") )</f>
+        <v xml:space="preserve">1.18 (0.83 - 1.69) </v>
+      </c>
+      <c r="G10" s="7" t="str">
+        <f>_xlfn.CONCAT(ROUND(eICU!V3, 2), " (", ROUND(eICU!V4,2), " - ", ROUND(eICU!V5,2),  ")",, IF(AND(eICU!V6 &lt;0.05, NOT(ISBLANK(eICU!V6))), "*", " ") )</f>
+        <v xml:space="preserve">0 (0 - 0) </v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>